<commit_message>
added tenant columns and links
</commit_message>
<xml_diff>
--- a/rx_PSC_UnitDirectory.xlsx
+++ b/rx_PSC_UnitDirectory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-UnitDirectory-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230B49C2-D4AD-4EE4-BF98-3FD3887EAE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D8A6D6-4218-45A0-B093-58D3A2579E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="570" windowWidth="28770" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Unit Directory</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Deposit</t>
-  </si>
-  <si>
     <t>Attributes</t>
   </si>
   <si>
@@ -55,15 +52,9 @@
     <t>Mkt Rent</t>
   </si>
   <si>
-    <t>Walk Thru Order</t>
-  </si>
-  <si>
     <t>Days Vacant</t>
   </si>
   <si>
-    <t>&amp;=display.PropertyName</t>
-  </si>
-  <si>
     <t>&amp;=display.UnitCode</t>
   </si>
   <si>
@@ -76,15 +67,9 @@
     <t>&amp;=display.Rent</t>
   </si>
   <si>
-    <t>&amp;=display.Deposit</t>
-  </si>
-  <si>
     <t>&amp;=display.Attributes</t>
   </si>
   <si>
-    <t>&amp;=display.WalkOrder</t>
-  </si>
-  <si>
     <t>&amp;=display.IsRentReady</t>
   </si>
   <si>
@@ -98,6 +83,30 @@
   </si>
   <si>
     <t>Rent Ready</t>
+  </si>
+  <si>
+    <t>&amp;=display.residentid</t>
+  </si>
+  <si>
+    <t>&amp;=display.Tenant_Full_Name</t>
+  </si>
+  <si>
+    <t>&amp;=display.OutputType</t>
+  </si>
+  <si>
+    <t>Tenant Code</t>
+  </si>
+  <si>
+    <t>&amp;=display.Tenant_Code</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=HYPERLINK(IF(O{r}="SCREEN", "javascript:DrillDown('../pages/TenantSwitch.aspx?TenantId="&amp;P{r}&amp;"')",""),Q{r})</t>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+  </si>
+  <si>
+    <t>&amp;=display.Property_Code</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -227,14 +236,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,59 +565,60 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
     <col min="4" max="4" width="8.453125" customWidth="1"/>
     <col min="5" max="5" width="7.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" customWidth="1"/>
-    <col min="7" max="7" width="32.26953125" customWidth="1"/>
-    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
     <col min="10" max="10" width="9.453125" customWidth="1"/>
     <col min="11" max="11" width="10.36328125" customWidth="1"/>
     <col min="12" max="12" width="21.36328125" customWidth="1"/>
+    <col min="15" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -613,72 +626,81 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="O4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +715,7 @@
     <oddFooter>&amp;C&amp;B Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1 A3:B3 D3 F3:G3 I3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A3:B3 D3 F3 I3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added date and bottom row border
</commit_message>
<xml_diff>
--- a/rx_PSC_UnitDirectory.xlsx
+++ b/rx_PSC_UnitDirectory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-UnitDirectory-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D8A6D6-4218-45A0-B093-58D3A2579E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC1DA56-2496-4FF0-B95E-E981F235ACF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="570" windowWidth="28770" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Unit Directory</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>&amp;=display.Property_Code</t>
+  </si>
+  <si>
+    <t>&amp;=display.ReportDateRange</t>
   </si>
 </sst>
 </file>
@@ -135,14 +138,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -162,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -191,6 +193,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="2" tint="-9.9978637043366805E-2"/>
       </left>
@@ -198,7 +211,9 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -211,6 +226,26 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -218,35 +253,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +604,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -589,34 +628,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -656,14 +697,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:17" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -672,36 +713,41 @@
       <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="M4" s="12"/>
+      <c r="O4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="2" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
attempting to not duplicate rows
</commit_message>
<xml_diff>
--- a/rx_PSC_UnitDirectory.xlsx
+++ b/rx_PSC_UnitDirectory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-UnitDirectory-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265DC88F-7863-4107-B642-E2B24E72CF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F1EFEC-0742-4375-9D05-6A98ACDEA478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Unit Directory</t>
   </si>
@@ -58,58 +58,61 @@
     <t>&amp;=display.UnitCode</t>
   </si>
   <si>
+    <t>&amp;=display.Area</t>
+  </si>
+  <si>
+    <t>&amp;=display.Rent</t>
+  </si>
+  <si>
+    <t>&amp;=display.Attributes</t>
+  </si>
+  <si>
+    <t>&amp;=display.IsRentReady</t>
+  </si>
+  <si>
+    <t>&amp;=display.UnitStatusDisplay</t>
+  </si>
+  <si>
+    <t>&amp;=display.DaysVacant</t>
+  </si>
+  <si>
+    <t>&amp;=display.Discount_Desc</t>
+  </si>
+  <si>
+    <t>Rent Ready</t>
+  </si>
+  <si>
+    <t>&amp;=display.residentid</t>
+  </si>
+  <si>
+    <t>&amp;=display.Tenant_Full_Name</t>
+  </si>
+  <si>
+    <t>&amp;=display.OutputType</t>
+  </si>
+  <si>
+    <t>Tenant Code</t>
+  </si>
+  <si>
+    <t>&amp;=display.Tenant_Code</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=HYPERLINK(IF(O{r}="SCREEN", "javascript:DrillDown('../pages/TenantSwitch.aspx?TenantId="&amp;P{r}&amp;"')",""),Q{r})</t>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+  </si>
+  <si>
+    <t>&amp;=display.Property_Code</t>
+  </si>
+  <si>
+    <t>&amp;=header.ReportDateRange</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=IF(ISNUMBER(MATCH(INDIRECT(ADDRESS(ROW(), COLUMN()-1)), INDIRECT(ADDRESS(ROW()-1, COLUMN()-1)), 0)), 0, 1)</t>
+  </si>
+  <si>
     <t>&amp;=display.UnitType</t>
-  </si>
-  <si>
-    <t>&amp;=display.Area</t>
-  </si>
-  <si>
-    <t>&amp;=display.Rent</t>
-  </si>
-  <si>
-    <t>&amp;=display.Attributes</t>
-  </si>
-  <si>
-    <t>&amp;=display.IsRentReady</t>
-  </si>
-  <si>
-    <t>&amp;=display.UnitStatusDisplay</t>
-  </si>
-  <si>
-    <t>&amp;=display.DaysVacant</t>
-  </si>
-  <si>
-    <t>&amp;=display.Discount_Desc</t>
-  </si>
-  <si>
-    <t>Rent Ready</t>
-  </si>
-  <si>
-    <t>&amp;=display.residentid</t>
-  </si>
-  <si>
-    <t>&amp;=display.Tenant_Full_Name</t>
-  </si>
-  <si>
-    <t>&amp;=display.OutputType</t>
-  </si>
-  <si>
-    <t>Tenant Code</t>
-  </si>
-  <si>
-    <t>&amp;=display.Tenant_Code</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=HYPERLINK(IF(O{r}="SCREEN", "javascript:DrillDown('../pages/TenantSwitch.aspx?TenantId="&amp;P{r}&amp;"')",""),Q{r})</t>
-  </si>
-  <si>
-    <t>Tenant Name</t>
-  </si>
-  <si>
-    <t>&amp;=display.Property_Code</t>
-  </si>
-  <si>
-    <t>&amp;=header.ReportDateRange</t>
   </si>
 </sst>
 </file>
@@ -235,39 +238,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,161 +588,158 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="6.7265625" customWidth="1"/>
-    <col min="3" max="3" width="20.7265625" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" customWidth="1"/>
-    <col min="6" max="6" width="35.7265625" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" customWidth="1"/>
-    <col min="12" max="12" width="21.36328125" customWidth="1"/>
-    <col min="15" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" customWidth="1"/>
+    <col min="7" max="7" width="35.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.36328125" customWidth="1"/>
+    <col min="13" max="13" width="21.36328125" customWidth="1"/>
+    <col min="16" max="18" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="P4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="O4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="9" t="s">
+      <c r="R4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -749,7 +748,7 @@
     <oddFooter>&amp;C&amp;B Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1 A3:B3 D3 F3 I3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A3:B3 E3 G3 J3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>